<commit_message>
Minor changes for the screen level privileges, Helpdesk Privileges; Added a temporary story for the complete flow for institution creation > user creation > institution parameter setup Updated the test data for Automation2, demo and stageSA environments
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/UploadFile.xlsx
+++ b/src/main/resources/config/demo/TestData/UploadFile.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E074127\Documents\InstitutionParameterSetup\mi-iss-automation-ips\src\main\resources\config\demo\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7728"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="CERFileUploadInvalid" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -500,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,7 +525,7 @@
     <col min="12" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -556,7 +560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -585,7 +589,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -614,7 +618,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -643,7 +647,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -672,11 +676,6 @@
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -684,7 +683,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -705,7 +704,7 @@
     <col min="12" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -740,7 +739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -769,7 +768,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -800,7 +799,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -829,7 +828,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -858,7 +857,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -889,7 +888,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -918,7 +917,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -947,8 +946,6 @@
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>